<commit_message>
modified:   Changelog.py 	modified:   Course_Finder- Shahman.ipynb 	modified:   Data/CUHK Comp.xlsx 	modified:   Data/HKUST Comp.xlsx 	modified:   HomePage.py 	modified:   Issues.py
</commit_message>
<xml_diff>
--- a/Data/CUHK Comp.xlsx
+++ b/Data/CUHK Comp.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hkustconnect-my.sharepoint.com/personal/saliac_connect_ust_hk/Documents/Uni/Course Database/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hkustconnect-my.sharepoint.com/personal/saliac_connect_ust_hk/Documents/Uni/Course Database/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45BD89DB-34BE-40C1-89AC-89F23EB7A1E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
@@ -1118,7 +1118,7 @@
   <dimension ref="A1:D85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>